<commit_message>
IMPROVE; POSs Transactions data
</commit_message>
<xml_diff>
--- a/src/POSsTransactions/assets/pos-transactions.xlsx
+++ b/src/POSsTransactions/assets/pos-transactions.xlsx
@@ -263,14 +263,14 @@
   <dimension ref="A1:DE14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="CV3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="CV1" activeCellId="0" sqref="CV1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="DA17" activeCellId="0" sqref="DA17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.51"/>
@@ -598,15 +598,9 @@
       <c r="DB2" s="2" t="n">
         <v>44805</v>
       </c>
-      <c r="DC2" s="2" t="n">
-        <v>44835</v>
-      </c>
-      <c r="DD2" s="2" t="n">
-        <v>44866</v>
-      </c>
-      <c r="DE2" s="2" t="n">
-        <v>44896</v>
-      </c>
+      <c r="DC2" s="2"/>
+      <c r="DD2" s="2"/>
+      <c r="DE2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">

</xml_diff>